<commit_message>
output folder path has changed to onedrive address
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kr\Documents\UiPath\GSS-\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophie J He\code\GSS-\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F88E1DC-396F-4870-A111-D35F92DCEFB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E8A430-783E-4777-8B92-0020ED476254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1218,10 +1218,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>C:\rpa\Output</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>PWCMiningTax</t>
   </si>
   <si>
@@ -1256,6 +1252,9 @@
   </si>
   <si>
     <t>C:\RPA\Log_output.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\Sophie J He\OneDrive - PwC China\RPA\Output</t>
   </si>
 </sst>
 </file>
@@ -1351,8 +1350,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1368,7 +1367,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2739,8 +2738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z986"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2877,7 +2876,7 @@
         <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -2885,7 +2884,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -2938,7 +2937,7 @@
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>388</v>
@@ -2946,10 +2945,10 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3933,8 +3932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39581073-175F-4128-A675-A220462453DE}">
   <dimension ref="A1:B173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="O114" sqref="O114"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>